<commit_message>
update : fix to convert 40x30 (heightxwidth) bin format
</commit_message>
<xml_diff>
--- a/performance_report.xlsx
+++ b/performance_report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>구분</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -208,12 +208,25 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>4phase/
+0318only</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>0318/0319/0320 에 적용
+no weights  (03-21 버전과 동등이상 임)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>4phase</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">0320까지 모든 데이터 적용
-no weights </t>
+    <t>incorrect_20200512_v3_28000_0318</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>incorrect_20200512_v3_all_data</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -624,16 +637,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -648,14 +685,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -665,39 +711,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -982,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L27"/>
+  <dimension ref="A2:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1002,23 +1015,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="A2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="5" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -1051,29 +1064,29 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
       <c r="K7" s="37"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="16">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22">
         <v>43963</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>39</v>
+      <c r="C8" s="24" t="s">
+        <v>41</v>
       </c>
       <c r="D8" s="1">
         <v>21365</v>
@@ -1085,49 +1098,50 @@
         <v>0</v>
       </c>
       <c r="G8" s="14">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ref="H8:H9" si="0">1-(G8/D8)</f>
-        <v>0.99962555581558621</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="22" t="s">
+        <v>0.99854902878539664</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="30" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="4">
+        <f>24969+63</f>
         <v>25032</v>
       </c>
-      <c r="E9" s="19"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="15">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="0"/>
-        <v>0.99952061361457334</v>
-      </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="23"/>
+        <v>0.99748322147651003</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="J9" s="31"/>
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="16">
-        <v>43911</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>35</v>
+      <c r="A10" s="20"/>
+      <c r="B10" s="22">
+        <v>43963</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="D10" s="1">
         <v>3500</v>
@@ -1139,52 +1153,52 @@
         <v>0</v>
       </c>
       <c r="G10" s="14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ref="H10:H27" si="1">1-(G10/D10)</f>
-        <v>0.99771428571428566</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>36</v>
+        <f t="shared" ref="H10:H11" si="1">1-(G10/D10)</f>
+        <v>0.99971428571428567</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="4">
         <v>3002</v>
       </c>
-      <c r="E11" s="19"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="G11" s="15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="1"/>
-        <v>0.99600266489007327</v>
-      </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="23"/>
+        <v>0.9956695536309127</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="16">
-        <v>43910</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>2</v>
+      <c r="A12" s="20"/>
+      <c r="B12" s="22">
+        <v>43911</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="1">
-        <v>21365</v>
+        <v>3500</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>33</v>
@@ -1193,330 +1207,342 @@
         <v>0</v>
       </c>
       <c r="G12" s="14">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99887666744675874</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="8">
-        <v>48</v>
-      </c>
+        <f t="shared" ref="H12:H29" si="2">1-(G12/D12)</f>
+        <v>0.99771428571428566</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="4">
-        <v>25032</v>
-      </c>
-      <c r="E13" s="19"/>
+        <v>3002</v>
+      </c>
+      <c r="E13" s="25"/>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="G13" s="15">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="1"/>
-        <v>0.99792265899648447</v>
-      </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="23"/>
+        <f t="shared" si="2"/>
+        <v>0.99600266489007327</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="31"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="16">
-        <v>43908</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22">
+        <v>43910</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>21365</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
-      <c r="G14" s="1">
-        <v>83</v>
+      <c r="G14" s="14">
+        <v>24</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99611514158670722</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" t="s">
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>0.99887666744675874</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="8">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="4">
         <v>25032</v>
       </c>
-      <c r="E15" s="19"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="4">
         <v>1</v>
       </c>
-      <c r="G15" s="12">
-        <v>24</v>
+      <c r="G15" s="15">
+        <v>52</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="1"/>
-        <v>0.99904122722914668</v>
-      </c>
-      <c r="I15" s="19"/>
+        <f t="shared" si="2"/>
+        <v>0.99792265899648447</v>
+      </c>
+      <c r="I15" s="29"/>
       <c r="J15" s="31"/>
-      <c r="K15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" t="s">
-        <v>26</v>
-      </c>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="16">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22">
         <v>43908</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="1">
         <v>21365</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
-      <c r="G16" s="11">
-        <v>37</v>
+      <c r="G16" s="1">
+        <v>83</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99826819564708635</v>
+        <f t="shared" si="2"/>
+        <v>0.99611514158670722</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="K16" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="L16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="4">
         <v>25032</v>
       </c>
-      <c r="E17" s="19"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="G17" s="4">
-        <v>127</v>
+      <c r="G17" s="12">
+        <v>24</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="1"/>
-        <v>0.99492649408756795</v>
-      </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="6"/>
+        <f t="shared" si="2"/>
+        <v>0.99904122722914668</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="L17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="16">
+      <c r="A18" s="20"/>
+      <c r="B18" s="22">
         <v>43908</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="1">
         <v>21365</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
       </c>
-      <c r="G18" s="10">
-        <v>11</v>
+      <c r="G18" s="11">
+        <v>37</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99948513924643112</v>
+        <f t="shared" si="2"/>
+        <v>0.99826819564708635</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>38</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="4">
         <v>25032</v>
       </c>
-      <c r="E19" s="19"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="4">
         <v>1</v>
       </c>
       <c r="G19" s="4">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="1"/>
-        <v>0.9955656759348035</v>
-      </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="31"/>
+        <f t="shared" si="2"/>
+        <v>0.99492649408756795</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="35"/>
       <c r="K19" s="6"/>
       <c r="L19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="27">
-        <v>43897</v>
-      </c>
-      <c r="C20" s="16" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="22">
+        <v>43908</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="1">
         <v>21365</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="1">
-        <v>138</v>
+      <c r="G20" s="10">
+        <v>11</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.9935408378188626</v>
+        <f t="shared" si="2"/>
+        <v>0.99948513924643112</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" s="3">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="17"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="4">
         <v>25032</v>
       </c>
-      <c r="E21" s="19"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="13">
-        <v>101</v>
+      <c r="G21" s="4">
+        <v>111</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="1"/>
-        <v>0.99596516458932571</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="6">
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>0.9955656759348035</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="6"/>
+      <c r="L21" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="38">
+        <v>43897</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="1">
         <v>21365</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F22" s="1">
         <v>0</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1">
+        <v>138</v>
+      </c>
       <c r="H22" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="3"/>
+        <f t="shared" si="2"/>
+        <v>0.9935408378188626</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="3">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="4">
         <v>25032</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="13">
+        <v>101</v>
+      </c>
       <c r="H23" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="6"/>
+        <f t="shared" si="2"/>
+        <v>0.99596516458932571</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="1">
@@ -1528,7 +1554,7 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I24" s="18"/>
@@ -1536,29 +1562,29 @@
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="4">
         <v>25032</v>
       </c>
-      <c r="E25" s="19"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="4">
         <v>1</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="1">
@@ -1570,7 +1596,7 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I26" s="18"/>
@@ -1578,98 +1604,146 @@
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="4">
         <v>25032</v>
       </c>
-      <c r="E27" s="19"/>
+      <c r="E27" s="25"/>
       <c r="F27" s="4">
         <v>1</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
       <c r="K27" s="6"/>
     </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>21365</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="4">
+        <v>25032</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B6:B7"/>
+  <mergeCells count="77">
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="I22:I23"/>
     <mergeCell ref="J22:J23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="I24:I25"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="I20:I21"/>
     <mergeCell ref="J20:J21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="J12:J13"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>